<commit_message>
ATEENDIGO- 7 + 8 + 9
</commit_message>
<xml_diff>
--- a/1. Login_eSign.xlsx
+++ b/1. Login_eSign.xlsx
@@ -5,21 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fendy.tio\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fendy.tio\Katalon Studio\ATeSign\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4575"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Setting" sheetId="2" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Url</t>
   </si>
@@ -85,6 +86,18 @@
   </si>
   <si>
     <t>AdIns2021</t>
+  </si>
+  <si>
+    <t>checkStoreDB</t>
+  </si>
+  <si>
+    <t>checkPaging</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -413,9 +426,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:B2">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>